<commit_message>
Add breeding probilities for 1540-1730 Set historical breeding probability to 0.35
</commit_message>
<xml_diff>
--- a/data/breedingprobability.xlsx
+++ b/data/breedingprobability.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Software\PopulationFitness\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D193E61B-FBD5-4B70-B361-FCFB952BF9B9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{F5025207-FABC-4751-8568-7FFF9B29C990}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" xr2:uid="{B15A1D60-9BBF-427E-9073-66A0D068863C}"/>
   </bookViews>
@@ -175,77 +175,92 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$24</c:f>
+              <c:f>Sheet1!$A$2:$A$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="23"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
+                  <c:v>1523</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1542</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1561</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1601</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1651</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>1701</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="6">
                   <c:v>1802</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="7">
                   <c:v>1812</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="8">
                   <c:v>1822</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="9">
                   <c:v>1832</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="10">
                   <c:v>1842</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="11">
                   <c:v>1852</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="12">
                   <c:v>1862</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="13">
                   <c:v>1872</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="14">
                   <c:v>1882</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="15">
                   <c:v>1892</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="16">
                   <c:v>1902</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="17">
                   <c:v>1912</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="18">
                   <c:v>1922</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="19">
                   <c:v>1932</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="20">
                   <c:v>1942</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="21">
                   <c:v>1952</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="22">
                   <c:v>1962</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="23">
                   <c:v>1972</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="24">
                   <c:v>1982</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="25">
                   <c:v>1992</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="26">
                   <c:v>2002</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="27">
                   <c:v>2012</c:v>
                 </c:pt>
               </c:numCache>
@@ -253,78 +268,93 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$24</c:f>
+              <c:f>Sheet1!$B$2:$B$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="23"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.31</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.38</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.37</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.41</c:v>
+                  <c:v>0.28999999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.43</c:v>
+                  <c:v>0.26</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.48</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.31</c:v>
+                  <c:v>0.28000000000000003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.33</c:v>
+                  <c:v>0.28000000000000003</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.34</c:v>
+                  <c:v>0.26</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.3</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>0.25</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.26</c:v>
-                </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.2</c:v>
+                  <c:v>0.22</c:v>
                 </c:pt>
                 <c:pt idx="13">
+                  <c:v>0.21</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.19</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.13</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.14000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>0.12</c:v>
                 </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.09</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.12</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.08</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.09</c:v>
-                </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.08</c:v>
+                  <c:v>7.0000000000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0.08</c:v>
                 </c:pt>
                 <c:pt idx="21">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="23">
                   <c:v>7.0000000000000007E-2</c:v>
                 </c:pt>
-                <c:pt idx="22">
-                  <c:v>7.0000000000000007E-2</c:v>
+                <c:pt idx="24">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.09</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -352,7 +382,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2012"/>
-          <c:min val="1701"/>
+          <c:min val="1523"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1081,13 +1111,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>47624</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>138112</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>609599</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>23812</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1413,10 +1443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD0BCD01-4691-44E5-A002-9298B68694D6}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B24"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1431,167 +1461,167 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1701</v>
+        <v>1523</v>
       </c>
       <c r="B2">
-        <v>0.31</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1802</v>
+        <v>1542</v>
       </c>
       <c r="B3">
-        <v>0.38</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1812</v>
+        <v>1561</v>
       </c>
       <c r="B4">
-        <v>0.37</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1822</v>
+        <v>1601</v>
       </c>
       <c r="B5">
-        <v>0.41</v>
+        <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1832</v>
+        <v>1651</v>
       </c>
       <c r="B6">
-        <v>0.43</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1842</v>
+        <v>1701</v>
       </c>
       <c r="B7">
-        <v>0.48</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>1852</v>
+        <v>1802</v>
       </c>
       <c r="B8">
-        <v>0.31</v>
+        <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>1862</v>
+        <v>1812</v>
       </c>
       <c r="B9">
-        <v>0.33</v>
+        <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>1872</v>
+        <v>1822</v>
       </c>
       <c r="B10">
-        <v>0.34</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>1882</v>
+        <v>1832</v>
       </c>
       <c r="B11">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>1892</v>
+        <v>1842</v>
       </c>
       <c r="B12">
-        <v>0.25</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>1902</v>
+        <v>1852</v>
       </c>
       <c r="B13">
-        <v>0.26</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>1912</v>
+        <v>1862</v>
       </c>
       <c r="B14">
-        <v>0.2</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>1922</v>
+        <v>1872</v>
       </c>
       <c r="B15">
-        <v>0.12</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>1932</v>
+        <v>1882</v>
       </c>
       <c r="B16">
-        <v>0.09</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>1942</v>
+        <v>1892</v>
       </c>
       <c r="B17">
-        <v>0.1</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>1952</v>
+        <v>1902</v>
       </c>
       <c r="B18">
-        <v>0.12</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>1962</v>
+        <v>1912</v>
       </c>
       <c r="B19">
-        <v>0.08</v>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>1972</v>
+        <v>1922</v>
       </c>
       <c r="B20">
-        <v>0.09</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>1982</v>
+        <v>1932</v>
       </c>
       <c r="B21">
-        <v>0.08</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>1992</v>
+        <v>1942</v>
       </c>
       <c r="B22">
         <v>0.08</v>
@@ -1599,18 +1629,58 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>2002</v>
+        <v>1952</v>
       </c>
       <c r="B23">
-        <v>7.0000000000000007E-2</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
+        <v>1962</v>
+      </c>
+      <c r="B24">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1972</v>
+      </c>
+      <c r="B25">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1982</v>
+      </c>
+      <c r="B26">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1992</v>
+      </c>
+      <c r="B27">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>2002</v>
+      </c>
+      <c r="B28">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
         <v>2012</v>
       </c>
-      <c r="B24">
-        <v>7.0000000000000007E-2</v>
+      <c r="B29">
+        <v>0.09</v>
       </c>
     </row>
   </sheetData>

</xml_diff>